<commit_message>
Update the application with latest bathroom product compatibility information
Replaced data/Product Data.xlsx, attached_assets/Product Data_05_30_2025.xlsx with new data; created backup Product_Data_backup_20250530_173232.xlsx.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 8eb032dd-4714-4ea5-9617-df6d3ccd324d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/37398790-88f1-466d-b3c2-6562db5e4667.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Product Data_05_30_2025.xlsx
+++ b/attached_assets/Product Data_05_30_2025.xlsx
@@ -529,19 +529,19 @@
     <t>47.125</t>
   </si>
   <si>
+    <t>Zen</t>
+  </si>
+  <si>
+    <t>220100-501-001-000</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/american-bath-group/image/upload/c_fill,w_1260,h_1260/v1720021397/websites-product-info-and-content/neptune/product-info/temp-images/zen-alcove-base-wht-deco-temp-image.jpg</t>
+  </si>
+  <si>
+    <t>Zen 4836 - Alcove</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>Zen</t>
-  </si>
-  <si>
-    <t>220100-501-001-000</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/american-bath-group/image/upload/c_fill,w_1260,h_1260/v1720021397/websites-product-info-and-content/neptune/product-info/temp-images/zen-alcove-base-wht-deco-temp-image.jpg</t>
-  </si>
-  <si>
-    <t>Zen 4836 - Alcove</t>
   </si>
   <si>
     <t>220100-503-001-000</t>
@@ -14015,7 +14015,7 @@
         <v>156</v>
       </c>
       <c r="G30" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="H30" t="s">
         <v>78</v>
@@ -14039,7 +14039,7 @@
         <v>108</v>
       </c>
       <c r="O30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P30" t="s"/>
       <c r="Q30" t="s"/>
@@ -14048,16 +14048,16 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" t="s">
         <v>159</v>
-      </c>
-      <c r="B31" t="s">
-        <v>160</v>
       </c>
       <c r="C31" t="s">
         <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E31" t="s">
         <v>155</v>
@@ -14066,7 +14066,7 @@
         <v>156</v>
       </c>
       <c r="G31" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H31" t="s">
         <v>78</v>
@@ -14090,7 +14090,7 @@
         <v>108</v>
       </c>
       <c r="O31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P31" t="s"/>
       <c r="Q31" t="s"/>
@@ -14117,7 +14117,7 @@
         <v>156</v>
       </c>
       <c r="G32" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="H32" t="s">
         <v>78</v>
@@ -14141,7 +14141,7 @@
         <v>108</v>
       </c>
       <c r="O32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P32" t="s"/>
       <c r="Q32" t="s"/>
@@ -16310,7 +16310,7 @@
         <v>279</v>
       </c>
       <c r="G75" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H75" t="s">
         <v>280</v>
@@ -16334,7 +16334,7 @@
         <v>108</v>
       </c>
       <c r="O75" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P75" t="s"/>
       <c r="Q75" t="s"/>
@@ -16361,7 +16361,7 @@
         <v>279</v>
       </c>
       <c r="G76" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H76" t="s">
         <v>280</v>
@@ -16385,7 +16385,7 @@
         <v>108</v>
       </c>
       <c r="O76" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P76" t="s"/>
       <c r="Q76" t="s"/>
@@ -18401,7 +18401,7 @@
         <v>394</v>
       </c>
       <c r="G116" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H116" t="s">
         <v>70</v>
@@ -18425,7 +18425,7 @@
         <v>108</v>
       </c>
       <c r="O116" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P116" t="s"/>
       <c r="Q116" t="s"/>
@@ -18452,7 +18452,7 @@
         <v>394</v>
       </c>
       <c r="G117" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="H117" t="s">
         <v>70</v>
@@ -18476,7 +18476,7 @@
         <v>108</v>
       </c>
       <c r="O117" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P117" t="s"/>
       <c r="Q117" t="s"/>
@@ -19217,7 +19217,7 @@
         <v>394</v>
       </c>
       <c r="G132" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H132" t="s">
         <v>70</v>
@@ -19241,7 +19241,7 @@
         <v>108</v>
       </c>
       <c r="O132" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P132" t="s">
         <v>440</v>
@@ -24170,7 +24170,7 @@
         <v>108</v>
       </c>
       <c r="O225" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P225">
         <v/>
@@ -24184,7 +24184,7 @@
         <v>671</v>
       </c>
       <c r="B226" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C226" t="s">
         <v>83</v>
@@ -24223,7 +24223,7 @@
         <v>108</v>
       </c>
       <c r="O226" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P226">
         <v/>
@@ -24276,7 +24276,7 @@
         <v>108</v>
       </c>
       <c r="O227" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P227">
         <v/>
@@ -25934,7 +25934,7 @@
         <v>279</v>
       </c>
       <c r="G259" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H259" t="s">
         <v>100</v>
@@ -25958,7 +25958,7 @@
         <v>108</v>
       </c>
       <c r="O259" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P259" t="s"/>
       <c r="Q259" t="s"/>
@@ -25985,7 +25985,7 @@
         <v>279</v>
       </c>
       <c r="G260" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="H260" t="s">
         <v>100</v>
@@ -26009,7 +26009,7 @@
         <v>108</v>
       </c>
       <c r="O260" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P260" t="s"/>
       <c r="Q260" t="s"/>
@@ -26036,7 +26036,7 @@
         <v>279</v>
       </c>
       <c r="G261" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="H261" t="s">
         <v>100</v>
@@ -26060,7 +26060,7 @@
         <v>108</v>
       </c>
       <c r="O261" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P261" t="s"/>
       <c r="Q261" t="s"/>
@@ -26087,7 +26087,7 @@
         <v>279</v>
       </c>
       <c r="G262" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H262" t="s">
         <v>100</v>
@@ -26111,7 +26111,7 @@
         <v>108</v>
       </c>
       <c r="O262" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P262" t="s"/>
       <c r="Q262" t="s"/>
@@ -28637,7 +28637,7 @@
         <v>1028</v>
       </c>
       <c r="G312" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H312" t="s">
         <v>1050</v>
@@ -28688,7 +28688,7 @@
         <v>46</v>
       </c>
       <c r="G313" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H313" t="s">
         <v>1070</v>
@@ -28892,7 +28892,7 @@
         <v>1498</v>
       </c>
       <c r="G317" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H317" t="s">
         <v>483</v>
@@ -29198,7 +29198,7 @@
         <v>1110</v>
       </c>
       <c r="G323" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H323" t="s">
         <v>483</v>
@@ -29249,7 +29249,7 @@
         <v>1110</v>
       </c>
       <c r="G324" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H324" t="s">
         <v>611</v>
@@ -29351,7 +29351,7 @@
         <v>1662</v>
       </c>
       <c r="G326" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H326" t="s">
         <v>1663</v>
@@ -30320,7 +30320,7 @@
         <v>1170</v>
       </c>
       <c r="G345" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H345" t="s">
         <v>2253</v>
@@ -31187,7 +31187,7 @@
         <v>2927</v>
       </c>
       <c r="G362" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H362" t="s">
         <v>1070</v>
@@ -31391,7 +31391,7 @@
         <v>3001</v>
       </c>
       <c r="G366" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H366" t="s">
         <v>187</v>
@@ -31442,7 +31442,7 @@
         <v>3024</v>
       </c>
       <c r="G367" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H367" t="s">
         <v>1050</v>
@@ -31544,7 +31544,7 @@
         <v>1573</v>
       </c>
       <c r="G369" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H369" t="s">
         <v>3057</v>
@@ -31595,7 +31595,7 @@
         <v>1285</v>
       </c>
       <c r="G370" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H370" t="s">
         <v>2253</v>
@@ -31799,7 +31799,7 @@
         <v>1543</v>
       </c>
       <c r="G374" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H374" t="s">
         <v>280</v>
@@ -32207,7 +32207,7 @@
         <v>925</v>
       </c>
       <c r="G382" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H382" t="s">
         <v>3425</v>
@@ -32666,7 +32666,7 @@
         <v>1285</v>
       </c>
       <c r="G391" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H391" t="s">
         <v>3653</v>
@@ -56490,7 +56490,7 @@
         <v/>
       </c>
       <c r="H22" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="I22">
         <v/>

</xml_diff>